<commit_message>
Added a shit tone of new call fars
</commit_message>
<xml_diff>
--- a/AutoTuneData/V4UB/master_excel.xlsx
+++ b/AutoTuneData/V4UB/master_excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alond\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\GitHub\codegurubyteme\AutoTuneData\V4UB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AD04D2-9AEF-4AFE-AFE1-386BE8B0B2D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9267324E-DF0E-4B0C-99C4-62E264DCE133}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{91287A1C-3F21-41B3-9BEA-97C18E6DE5E0}"/>
   </bookViews>
@@ -928,7 +928,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1227,8 +1227,8 @@
   <dimension ref="A1:L259"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L259" sqref="L259"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L249" sqref="L249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>